<commit_message>
New update with updated scripts
</commit_message>
<xml_diff>
--- a/pipelin_pgms.xlsx
+++ b/pipelin_pgms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="24680" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="8060" yWindow="740" windowWidth="24820" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
   <si>
     <t>plot_coverage_chimeras_insertsize_contamination.R</t>
   </si>
@@ -72,15 +72,9 @@
     <t>insertion/deletion ratio per sample, N. of insertion, N. of deletion</t>
   </si>
   <si>
-    <t>plot_bcftools_stat.R</t>
-  </si>
-  <si>
     <t>% of the genome &gt; 30x per sample</t>
   </si>
   <si>
-    <t>DP_gt_30_by_sample.png</t>
-  </si>
-  <si>
     <t>Script 1</t>
   </si>
   <si>
@@ -96,123 +90,36 @@
     <t>Pipeline step</t>
   </si>
   <si>
-    <t>*.sexcheck</t>
-  </si>
-  <si>
-    <t>contamination_by_sample.png</t>
-  </si>
-  <si>
-    <t>coverage_by_sample.png</t>
-  </si>
-  <si>
-    <t>insert_size_distribution_by_sample.png</t>
-  </si>
-  <si>
-    <t>Measure</t>
-  </si>
-  <si>
-    <t>Plot</t>
-  </si>
-  <si>
-    <t>meanmedcoverage.csv</t>
-  </si>
-  <si>
-    <t>chimeras_by_sample.png</t>
-  </si>
-  <si>
-    <t>contamination.csv</t>
-  </si>
-  <si>
-    <t>chimeras.csv</t>
-  </si>
-  <si>
-    <t>medianinsert.csv</t>
-  </si>
-  <si>
-    <t>MDS.png</t>
-  </si>
-  <si>
-    <t>IBD_vs_zero_IBS_sharing.png</t>
-  </si>
-  <si>
-    <t>ReadPosRankSum_by_VQSRTranche.png</t>
-  </si>
-  <si>
-    <t>MQranksum_by_VQSRTranche.png</t>
-  </si>
-  <si>
-    <t>inbcoef_by_VQSRTranche.png</t>
-  </si>
-  <si>
-    <t>FS_by_VQSRTranche.png</t>
-  </si>
-  <si>
-    <t>DP_by_VQSRTranche.png</t>
-  </si>
-  <si>
-    <t>QD_by_VQSRTranche.png</t>
-  </si>
-  <si>
     <t>Base modifications</t>
   </si>
   <si>
-    <t>base_modifications.png</t>
-  </si>
-  <si>
-    <t>length_indel.png</t>
-  </si>
-  <si>
-    <t>insertionDeletionRatio_by_sample.png</t>
-  </si>
-  <si>
-    <t>GC content per sample</t>
-  </si>
-  <si>
     <t>Percentage of chimeric regions per sample</t>
   </si>
   <si>
     <t>Contamination estimates per sample</t>
   </si>
   <si>
-    <t>singeltons_by_sample.png</t>
-  </si>
-  <si>
     <t>Singeltons per sample</t>
   </si>
   <si>
     <t>N. variant loci per sample</t>
   </si>
   <si>
-    <t>nVariantLoci_by_sample.png</t>
-  </si>
-  <si>
-    <t>hetHomRatio_by_sample.png</t>
-  </si>
-  <si>
     <t>Ti/Tv  per sample</t>
   </si>
   <si>
-    <t>TITV_by_sample.png</t>
-  </si>
-  <si>
     <t>calculate_GQ_by_DP.py</t>
   </si>
   <si>
     <t>% of missin per sample</t>
   </si>
   <si>
-    <t>missing_by_sample.png</t>
-  </si>
-  <si>
     <t>plot_het_hardy_miss.R</t>
   </si>
   <si>
     <t>calculate_het_hardy_miss.sh</t>
   </si>
   <si>
-    <t>F_by_sample.png</t>
-  </si>
-  <si>
     <t>F stat for heterozygosity  per sample</t>
   </si>
   <si>
@@ -228,96 +135,30 @@
     <t>Mean sequencing depth per variant</t>
   </si>
   <si>
-    <t>GQ_MEAN_by_variant.png</t>
-  </si>
-  <si>
-    <t>DP_by_variant.png</t>
-  </si>
-  <si>
     <t>% of missing genotypes per variant</t>
   </si>
   <si>
-    <t>missing_by_variant.png</t>
-  </si>
-  <si>
-    <t>HWE_by_variant.png</t>
-  </si>
-  <si>
     <t>H-W P-value per variant</t>
   </si>
   <si>
-    <t>Ti/Tv by allele frequency per variant</t>
-  </si>
-  <si>
-    <t>plot_INFO_by_TI_TV_per_variant.R</t>
-  </si>
-  <si>
-    <t>Ti/Tv by DP per variant</t>
-  </si>
-  <si>
-    <t>Ti/Tv by VQSLOD per variant</t>
-  </si>
-  <si>
-    <t>TI_TV_by_AF.png</t>
-  </si>
-  <si>
-    <t>TI_TV_by_DP.png</t>
-  </si>
-  <si>
-    <t>TI_TV_by_VQSLOD.png</t>
-  </si>
-  <si>
     <t>DP by GQ per variant</t>
   </si>
   <si>
-    <t>DP_by_GQ_by_variant.png</t>
-  </si>
-  <si>
-    <t>allele_balance_by_variant.png</t>
-  </si>
-  <si>
     <t>Average allele balance per variant</t>
   </si>
   <si>
-    <t>calculate_allele_balance.sh</t>
-  </si>
-  <si>
-    <t>percent_bad_allele_balance_by_variant.png</t>
-  </si>
-  <si>
     <t>GQ &gt; 20 by DP per genotype</t>
   </si>
   <si>
-    <t>% of samples with alleles deviating the 20/80 read depth ratio</t>
-  </si>
-  <si>
-    <t>GQ_gt_20_by_DP.png</t>
-  </si>
-  <si>
     <t>General statistics about N. SNPs, INDELs, etc…</t>
   </si>
   <si>
-    <t>*.stats</t>
-  </si>
-  <si>
     <t>Mean/median coverage per sample</t>
   </si>
   <si>
     <t>plot_gatk_stat.R</t>
   </si>
   <si>
-    <t>N. of variants with GQ &lt; 20, but DP &gt; 30</t>
-  </si>
-  <si>
-    <t>Ti/Tv by allele count per variant</t>
-  </si>
-  <si>
-    <t>TI_TV_by_AC.png</t>
-  </si>
-  <si>
-    <t>GQ_lt_20_DP_gt_30_by_sample.png</t>
-  </si>
-  <si>
     <t>plot_DP_GQ_relation.R</t>
   </si>
   <si>
@@ -330,10 +171,49 @@
     <t>plot_concordance_WGS_chip.R</t>
   </si>
   <si>
-    <t>concordance_WG_chip_by_DP.png</t>
-  </si>
-  <si>
     <t>PCA overlap with exac data</t>
+  </si>
+  <si>
+    <t>calculate_GC_content.sh</t>
+  </si>
+  <si>
+    <t>plot_GC_content.R</t>
+  </si>
+  <si>
+    <t>GC and AT dropout per sample</t>
+  </si>
+  <si>
+    <t>Normalized coverage by GC windows per sample</t>
+  </si>
+  <si>
+    <t>calculate_GQ_DP_mean.sh</t>
+  </si>
+  <si>
+    <t>calculate_indel_length.sh</t>
+  </si>
+  <si>
+    <t>plot_base_changes.R</t>
+  </si>
+  <si>
+    <t>plot_indel_length.R</t>
+  </si>
+  <si>
+    <t>calculate_PCA_over_EXAC.sh</t>
+  </si>
+  <si>
+    <t>plot_pca_over_exac.R</t>
+  </si>
+  <si>
+    <t>calculate_DP_80_20_z_score.py</t>
+  </si>
+  <si>
+    <t>plot_allele_balance_stat_by_variant.R</t>
+  </si>
+  <si>
+    <t>Distribution of z score from testing P(ALT|DP,0.47) per sample</t>
+  </si>
+  <si>
+    <t>% of samples with  P(ALT|DP,0.47)  &lt; 0.05</t>
   </si>
 </sst>
 </file>
@@ -373,18 +253,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -396,7 +270,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -498,14 +372,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -556,6 +439,11 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -606,6 +494,11 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -935,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:D40"/>
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -947,69 +840,49 @@
     <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="56.1640625" customWidth="1"/>
     <col min="4" max="4" width="32.1640625" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1019,157 +892,130 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1">
-      <c r="A8" s="1">
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1">
+      <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1177,16 +1023,13 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -1194,16 +1037,13 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -1211,16 +1051,13 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -1228,16 +1065,13 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -1245,394 +1079,291 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
         <v>62</v>
       </c>
-      <c r="D26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
-      </c>
-      <c r="F34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
-      </c>
-      <c r="F36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" t="s">
-        <v>86</v>
-      </c>
-      <c r="F37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s">
-        <v>88</v>
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="1" customFormat="1">
+      <c r="A37" s="1">
+        <v>6</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
-      </c>
-      <c r="E38" t="s">
-        <v>99</v>
-      </c>
-      <c r="F38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="1" customFormat="1">
-      <c r="A39">
-        <v>5</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="1" customFormat="1">
-      <c r="A40" s="1">
-        <v>6</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="2">
-        <v>7</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" t="s">
-        <v>102</v>
-      </c>
-      <c r="F41" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>